<commit_message>
forign & company buying in a row function complete
</commit_message>
<xml_diff>
--- a/venv/AI_List.xlsx
+++ b/venv/AI_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijiu\Desktop\work\Git\Stock_simulation_work\venv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172B51DB-3B3A-4E88-ADB2-8D73847AC253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B5D36F-D2E4-484D-A65A-F884D6FC9ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9308FE10-FF23-4110-A9F6-220CDE366E5D}"/>
   </bookViews>
@@ -133,10 +133,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>신세계</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <r>
       <t>SK</t>
     </r>
@@ -168,31 +164,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <t>KB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="BatangChe"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>금융</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>메리츠화재</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>삼성전자</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>NAVER</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>휠라홀딩스</t>
+  </si>
+  <si>
+    <t>현대건설기계</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>대한항공</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -254,7 +241,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -280,6 +267,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -600,7 +590,7 @@
   <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -697,112 +687,112 @@
     </row>
     <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
-        <v>44116</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>44117</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="4">
-        <v>216000</v>
+        <v>240000</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>44117</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="4">
-        <v>240000</v>
+        <v>24700</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
-        <v>44117</v>
+        <v>44119</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="4">
-        <v>24700</v>
+        <v>23950</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
-        <v>44119</v>
+        <v>44120</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="4">
-        <v>23950</v>
+        <v>12550</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
-        <v>44120</v>
+        <v>44123</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="4">
-        <v>12550</v>
+        <v>25950</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
-        <v>44123</v>
+        <v>44124</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="4">
-        <v>25950</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+        <v>59500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
-        <v>44123</v>
+        <v>44124</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="4">
-        <v>40700</v>
+        <v>308875</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
-        <v>44124</v>
+        <v>44125</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="4">
-        <v>14300</v>
+        <v>40250</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
-        <v>44124</v>
+        <v>44126</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="4">
-        <v>59500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>44124</v>
-      </c>
-      <c r="B20" s="3" t="s">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>44127</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="4">
-        <v>308875</v>
+        <v>21300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>